<commit_message>
Added a test realisation of type scanner (files main.cpp and test.cpp)
</commit_message>
<xml_diff>
--- a/FromPlusesToAssemblyLab1/cmake-build-debug/xlsxFiles/Identifiers.xlsx
+++ b/FromPlusesToAssemblyLab1/cmake-build-debug/xlsxFiles/Identifiers.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>№</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t>ased</t>
-  </si>
-  <si>
-    <t>myVariable</t>
   </si>
   <si>
     <t>a</t>
@@ -369,7 +366,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -430,17 +427,6 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6">
-        <v>30</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0,7" right="0,7" top="0,75" bottom="0,75" header="0,3" footer="0,3"/>
 </worksheet>

</xml_diff>